<commit_message>
Aanpassingen BAG exelsheets voor upload
</commit_message>
<xml_diff>
--- a/catalogusdata/BAG/BegrippenExcel BAG T.xlsx
+++ b/catalogusdata/BAG/BegrippenExcel BAG T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\wsc20785\Documents\Projecten\Kadaster\Data\Bag handshake\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\LDT upload\catalogus\catalogusdata\BAG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="129">
   <si>
     <t>tabblad</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Gevalideerd</t>
   </si>
   <si>
-    <t>dataset:BagToelichtingsBegrip</t>
-  </si>
-  <si>
     <t>voorbeeld</t>
   </si>
   <si>
@@ -408,6 +405,12 @@
   </si>
   <si>
     <t>NEN 2580:2007, artikel 2.1.2: Een binnenruimte is een "ruimte die aan alle zijden volledig wordt begrensd door bouwkundige scheidingsconstructies."   Definitie overgenomen met toestemming van NEN te Delft.</t>
+  </si>
+  <si>
+    <t>BagToelichtingsBegrip</t>
+  </si>
+  <si>
+    <t>http://kadaster.basisregistraties.overheid.nl/som/def#{eigenschap}</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -486,7 +489,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -797,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,16 +923,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>89</v>
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -938,10 +940,13 @@
         <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -949,10 +954,10 @@
         <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -960,10 +965,10 @@
         <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -971,10 +976,10 @@
         <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -982,10 +987,10 @@
         <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -993,10 +998,10 @@
         <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,10 +1009,10 @@
         <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1015,24 +1020,21 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1040,24 +1042,24 @@
         <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,24 +1067,24 @@
         <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,14 +1092,25 @@
         <v>86</v>
       </c>
       <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" s="2"/>
@@ -1158,31 +1171,35 @@
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1"/>
     <hyperlink ref="D6" r:id="rId2" location="{eigenschap}"/>
-    <hyperlink ref="D11" r:id="rId3"/>
-    <hyperlink ref="D12" r:id="rId4"/>
-    <hyperlink ref="D13" r:id="rId5"/>
-    <hyperlink ref="D14" r:id="rId6"/>
-    <hyperlink ref="D15" r:id="rId7"/>
-    <hyperlink ref="D17" r:id="rId8"/>
-    <hyperlink ref="D18" r:id="rId9"/>
-    <hyperlink ref="D8" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId3"/>
+    <hyperlink ref="D13" r:id="rId4"/>
+    <hyperlink ref="D14" r:id="rId5"/>
+    <hyperlink ref="D15" r:id="rId6"/>
+    <hyperlink ref="D16" r:id="rId7"/>
+    <hyperlink ref="D18" r:id="rId8"/>
+    <hyperlink ref="D19" r:id="rId9"/>
+    <hyperlink ref="D9" r:id="rId10"/>
     <hyperlink ref="D7" r:id="rId11" location="{eigenschap}"/>
     <hyperlink ref="D2" r:id="rId12" location="{klasse}"/>
-    <hyperlink ref="D9" r:id="rId13" location="{subklasse}"/>
-    <hyperlink ref="D10" r:id="rId14"/>
-    <hyperlink ref="D22" r:id="rId15"/>
-    <hyperlink ref="D21" r:id="rId16"/>
-    <hyperlink ref="D19" r:id="rId17"/>
-    <hyperlink ref="D20" r:id="rId18"/>
-    <hyperlink ref="D16" r:id="rId19"/>
+    <hyperlink ref="D10" r:id="rId13" location="{subklasse}"/>
+    <hyperlink ref="D11" r:id="rId14"/>
+    <hyperlink ref="D23" r:id="rId15"/>
+    <hyperlink ref="D22" r:id="rId16"/>
+    <hyperlink ref="D20" r:id="rId17"/>
+    <hyperlink ref="D21" r:id="rId18"/>
+    <hyperlink ref="D17" r:id="rId19"/>
+    <hyperlink ref="D8" r:id="rId20" location="{eigenschap}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -1191,7 +1208,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,20 +1241,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1496,299 +1513,299 @@
         <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
         <v>107</v>
       </c>
-      <c r="E17" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>65</v>
       </c>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="54" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="54" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -1796,18 +1813,18 @@
       <c r="E54"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1819,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,30 +1903,30 @@
         <v>54</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="5"/>
       <c r="E2" s="3" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2"/>
       <c r="H2" t="s">
         <v>104</v>
       </c>
       <c r="I2"/>
-      <c r="J2" s="10">
+      <c r="J2" s="9">
         <v>42933</v>
       </c>
       <c r="K2" s="5"/>
@@ -1917,31 +1934,31 @@
       <c r="M2"/>
       <c r="N2" s="5"/>
       <c r="O2"/>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="7" t="s">
-        <v>105</v>
+      <c r="E3" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3"/>
       <c r="H3" t="s">
         <v>104</v>
       </c>
       <c r="I3" s="6"/>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>42933</v>
       </c>
       <c r="K3" s="5"/>
@@ -1950,27 +1967,27 @@
       <c r="N3" s="5"/>
       <c r="O3"/>
     </row>
-    <row r="4" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="8"/>
+      <c r="B4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G4"/>
       <c r="H4" t="s">
         <v>104</v>
       </c>
       <c r="I4"/>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>42933</v>
       </c>
       <c r="K4" s="5"/>
@@ -1979,27 +1996,27 @@
       <c r="N4" s="5"/>
       <c r="O4"/>
     </row>
-    <row r="5" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="C5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="3" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G5"/>
       <c r="H5" t="s">
         <v>104</v>
       </c>
       <c r="I5"/>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>42933</v>
       </c>
       <c r="K5" s="5"/>
@@ -2008,27 +2025,27 @@
       <c r="N5" s="5"/>
       <c r="O5"/>
     </row>
-    <row r="6" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="C6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="3" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
         <v>104</v>
       </c>
       <c r="I6"/>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>42933</v>
       </c>
       <c r="K6" s="5"/>
@@ -2037,17 +2054,17 @@
       <c r="N6" s="5"/>
       <c r="O6"/>
     </row>
-    <row r="7" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="C7"/>
       <c r="D7" s="5"/>
       <c r="E7" s="3" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
@@ -2055,7 +2072,7 @@
         <v>104</v>
       </c>
       <c r="I7"/>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>42933</v>
       </c>
       <c r="K7" s="5"/>
@@ -2063,31 +2080,31 @@
       <c r="M7"/>
       <c r="N7" s="5"/>
       <c r="O7"/>
-      <c r="P7" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="P7" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="C8"/>
       <c r="D8" s="5"/>
       <c r="E8" s="3" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
         <v>104</v>
       </c>
       <c r="I8"/>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>42933</v>
       </c>
       <c r="K8" s="5"/>
@@ -2096,27 +2113,27 @@
       <c r="N8" s="5"/>
       <c r="O8"/>
     </row>
-    <row r="9" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>98</v>
       </c>
       <c r="C9"/>
       <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G9"/>
       <c r="H9" t="s">
         <v>104</v>
       </c>
       <c r="I9"/>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>42933</v>
       </c>
       <c r="K9" s="5"/>
@@ -2125,7 +2142,7 @@
       <c r="N9" s="5"/>
       <c r="O9"/>
     </row>
-    <row r="10" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -2142,7 +2159,7 @@
       <c r="N10" s="5"/>
       <c r="O10"/>
     </row>
-    <row r="11" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -2159,7 +2176,7 @@
       <c r="N11" s="5"/>
       <c r="O11"/>
     </row>
-    <row r="12" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -2226,49 +2243,49 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="10"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="10"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="10"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="10"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="10"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="10"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="10"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="10"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="10"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="10"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="10"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="10"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="10"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="10"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="10"/>
+      <c r="D20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2317,19 +2334,19 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="10"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="10"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="10"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="10"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="10"/>
+      <c r="C12" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>